<commit_message>
mostly done with dropping data
</commit_message>
<xml_diff>
--- a/feature_description.xlsx
+++ b/feature_description.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cynthiax/Desktop/DATA1030/data1030-load-default-prob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15AE2E-D931-B840-A802-8B4BD8B8C388}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4941E5C-2377-9246-97A2-3CCC352419B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14960" yWindow="1060" windowWidth="17540" windowHeight="15080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStatsFull" sheetId="2" r:id="rId1"/>
     <sheet name="LoanStats_&lt;20%missingval" sheetId="3" r:id="rId2"/>
+    <sheet name="LoanStats_final" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="307">
   <si>
     <t>acc_now_delinq</t>
   </si>
@@ -2679,8 +2679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E244C6-A244-CB45-901D-7855F447B1B1}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3526,4 +3526,413 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E15306-1EC0-7149-BCA9-9E710C9AE138}">
+  <dimension ref="A1:K45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+      <c r="B45" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>